<commit_message>
Primeiro commit do dashboard de defeitos
</commit_message>
<xml_diff>
--- a/PythonProject/App/dados/Defeitos abertos Maio e Junho 2025.xlsx
+++ b/PythonProject/App/dados/Defeitos abertos Maio e Junho 2025.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karenaol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regina\dashboard-defeitos-funcionais\PythonProject\App\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA174292-0329-45DA-8F4F-1D9046A6D598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados!$A$1:$B$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
@@ -255,7 +254,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
@@ -410,12 +409,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma" xfId="4"/>
+    <cellStyle name="Comma [0]" xfId="5"/>
+    <cellStyle name="Currency" xfId="2"/>
+    <cellStyle name="Currency [0]" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Percent" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -431,7 +430,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Kauan Arena Oliveira" refreshedDate="45821.729537615742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{4EFD4F1F-62D7-4354-AE5A-69477EE7E0E0}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kauan Arena Oliveira" refreshedDate="45821.729537615742" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G50" sheet="Dados"/>
   </cacheSource>
@@ -1862,7 +1861,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4D89FB87-9A0E-45E8-985B-FB7FE6DC58C2}" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B109" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -3489,26 +3488,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38A8BFE-915F-4BE3-92E2-B08BE1611E81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="114" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3534,7 +3533,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>21304</v>
       </c>
@@ -3557,11 +3556,11 @@
         <v>6</v>
       </c>
       <c r="H2">
-        <f>IF(AND(E2&lt;&gt;"",F2&lt;&gt;""),F2-E2+1,0)</f>
+        <f ca="1">IF(E2&lt;&gt;"",IF(F2&lt;&gt;"",F2,TODAY())-E2+1,0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>21366</v>
       </c>
@@ -3582,11 +3581,11 @@
         <v>16</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H50" si="0">IF(AND(E3&lt;&gt;"",F3&lt;&gt;""),F3-E3+1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H3:H50" ca="1" si="0">IF(E3&lt;&gt;"",IF(F3&lt;&gt;"",F3,TODAY())-E3+1,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>21289</v>
       </c>
@@ -3609,11 +3608,11 @@
         <v>6</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>21295</v>
       </c>
@@ -3634,11 +3633,11 @@
         <v>7</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>21355</v>
       </c>
@@ -3661,11 +3660,11 @@
         <v>7</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>21279</v>
       </c>
@@ -3688,11 +3687,11 @@
         <v>6</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>21306</v>
       </c>
@@ -3715,11 +3714,11 @@
         <v>7</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>21363</v>
       </c>
@@ -3742,11 +3741,11 @@
         <v>7</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>21356</v>
       </c>
@@ -3769,11 +3768,11 @@
         <v>6</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>21302</v>
       </c>
@@ -3796,11 +3795,11 @@
         <v>6</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>21284</v>
       </c>
@@ -3823,11 +3822,11 @@
         <v>6</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>21360</v>
       </c>
@@ -3850,11 +3849,11 @@
         <v>6</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>21276</v>
       </c>
@@ -3877,11 +3876,11 @@
         <v>6</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>21365</v>
       </c>
@@ -3902,11 +3901,11 @@
         <v>6</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>21275</v>
       </c>
@@ -3929,11 +3928,11 @@
         <v>6</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>21290</v>
       </c>
@@ -3956,11 +3955,11 @@
         <v>6</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>21274</v>
       </c>
@@ -3983,11 +3982,11 @@
         <v>6</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>21294</v>
       </c>
@@ -4010,11 +4009,11 @@
         <v>6</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>21273</v>
       </c>
@@ -4037,11 +4036,11 @@
         <v>6</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>21286</v>
       </c>
@@ -4064,11 +4063,11 @@
         <v>6</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>21272</v>
       </c>
@@ -4091,11 +4090,11 @@
         <v>6</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>21285</v>
       </c>
@@ -4118,11 +4117,11 @@
         <v>7</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>21315</v>
       </c>
@@ -4145,11 +4144,11 @@
         <v>6</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>21311</v>
       </c>
@@ -4172,11 +4171,11 @@
         <v>7</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>21350</v>
       </c>
@@ -4199,11 +4198,11 @@
         <v>6</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>21314</v>
       </c>
@@ -4226,11 +4225,11 @@
         <v>6</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>21313</v>
       </c>
@@ -4253,11 +4252,11 @@
         <v>6</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>21361</v>
       </c>
@@ -4280,11 +4279,11 @@
         <v>6</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>21329</v>
       </c>
@@ -4305,11 +4304,11 @@
         <v>7</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
         <v>21326</v>
       </c>
@@ -4332,11 +4331,11 @@
         <v>6</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
         <v>21352</v>
       </c>
@@ -4359,11 +4358,11 @@
         <v>7</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
         <v>21330</v>
       </c>
@@ -4386,11 +4385,11 @@
         <v>6</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>21325</v>
       </c>
@@ -4413,11 +4412,11 @@
         <v>6</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <v>21337</v>
       </c>
@@ -4440,11 +4439,11 @@
         <v>6</v>
       </c>
       <c r="H35">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
         <v>21332</v>
       </c>
@@ -4467,11 +4466,11 @@
         <v>6</v>
       </c>
       <c r="H36">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <v>21322</v>
       </c>
@@ -4494,11 +4493,11 @@
         <v>6</v>
       </c>
       <c r="H37">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
         <v>21354</v>
       </c>
@@ -4521,11 +4520,11 @@
         <v>7</v>
       </c>
       <c r="H38">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="10">
         <v>21319</v>
       </c>
@@ -4548,11 +4547,11 @@
         <v>7</v>
       </c>
       <c r="H39">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <v>21318</v>
       </c>
@@ -4575,11 +4574,11 @@
         <v>7</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <v>21320</v>
       </c>
@@ -4602,11 +4601,11 @@
         <v>7</v>
       </c>
       <c r="H41">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
         <v>21358</v>
       </c>
@@ -4629,11 +4628,11 @@
         <v>6</v>
       </c>
       <c r="H42">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="10">
         <v>21357</v>
       </c>
@@ -4656,11 +4655,11 @@
         <v>6</v>
       </c>
       <c r="H43">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
         <v>21368</v>
       </c>
@@ -4681,11 +4680,11 @@
         <v>7</v>
       </c>
       <c r="H44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
         <v>21367</v>
       </c>
@@ -4706,11 +4705,11 @@
         <v>6</v>
       </c>
       <c r="H45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
         <v>21364</v>
       </c>
@@ -4731,11 +4730,11 @@
         <v>6</v>
       </c>
       <c r="H46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="10">
         <v>21362</v>
       </c>
@@ -4756,11 +4755,11 @@
         <v>7</v>
       </c>
       <c r="H47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
         <v>21370</v>
       </c>
@@ -4783,11 +4782,11 @@
         <v>7</v>
       </c>
       <c r="H48">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="10">
         <v>21369</v>
       </c>
@@ -4810,11 +4809,11 @@
         <v>6</v>
       </c>
       <c r="H49">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="14">
         <v>21371</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>6</v>
       </c>
       <c r="H50">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -4847,59 +4846,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648E5C34-583C-40CF-87BF-72F7DE5D6530}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:B109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="123.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="123.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="23" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="23" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="23" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="23" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="23" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="23" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="23" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="23" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="23" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="23" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="28" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="12" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="12" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="12" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="12" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>57</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -4915,7 +4914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
@@ -4923,7 +4922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>21304</v>
       </c>
@@ -4931,7 +4930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -4939,7 +4938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>50</v>
       </c>
@@ -4947,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>21366</v>
       </c>
@@ -4955,7 +4954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -4971,7 +4970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>21289</v>
       </c>
@@ -4979,7 +4978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>62</v>
       </c>
@@ -4987,7 +4986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
@@ -4995,7 +4994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>21295</v>
       </c>
@@ -5003,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
@@ -5019,7 +5018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>21272</v>
       </c>
@@ -5027,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>21285</v>
       </c>
@@ -5035,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>55</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>21286</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>23</v>
       </c>
@@ -5059,7 +5058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>21273</v>
       </c>
@@ -5067,7 +5066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>27</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>21294</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>21</v>
       </c>
@@ -5091,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>21274</v>
       </c>
@@ -5099,7 +5098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>26</v>
       </c>
@@ -5107,7 +5106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>21290</v>
       </c>
@@ -5115,7 +5114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>20</v>
       </c>
@@ -5123,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>21275</v>
       </c>
@@ -5131,7 +5130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>49</v>
       </c>
@@ -5139,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="8">
         <v>21365</v>
       </c>
@@ -5147,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
@@ -5155,7 +5154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>21276</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>45</v>
       </c>
@@ -5171,7 +5170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>21360</v>
       </c>
@@ -5179,7 +5178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>24</v>
       </c>
@@ -5187,7 +5186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="8">
         <v>21284</v>
       </c>
@@ -5195,7 +5194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>21302</v>
       </c>
@@ -5203,7 +5202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>41</v>
       </c>
@@ -5211,7 +5210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>21356</v>
       </c>
@@ -5219,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>18</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>21279</v>
       </c>
@@ -5235,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="8">
         <v>21306</v>
       </c>
@@ -5243,7 +5242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>21355</v>
       </c>
@@ -5251,7 +5250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>21363</v>
       </c>
@@ -5259,7 +5258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>10</v>
       </c>
@@ -5267,7 +5266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>29</v>
       </c>
@@ -5275,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>21311</v>
       </c>
@@ -5283,7 +5282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>31</v>
       </c>
@@ -5291,7 +5290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>21315</v>
       </c>
@@ -5299,7 +5298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>11</v>
       </c>
@@ -5307,7 +5306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>19</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>21313</v>
       </c>
@@ -5323,7 +5322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>30</v>
       </c>
@@ -5331,7 +5330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>21314</v>
       </c>
@@ -5339,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>40</v>
       </c>
@@ -5347,7 +5346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>21350</v>
       </c>
@@ -5355,7 +5354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>12</v>
       </c>
@@ -5363,7 +5362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>32</v>
       </c>
@@ -5371,7 +5370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>21320</v>
       </c>
@@ -5379,7 +5378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>29</v>
       </c>
@@ -5387,7 +5386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>21318</v>
       </c>
@@ -5395,7 +5394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>56</v>
       </c>
@@ -5403,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="8">
         <v>21319</v>
       </c>
@@ -5411,7 +5410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>42</v>
       </c>
@@ -5419,7 +5418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>21354</v>
       </c>
@@ -5427,7 +5426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>34</v>
       </c>
@@ -5435,7 +5434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="8">
         <v>21322</v>
       </c>
@@ -5443,7 +5442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>36</v>
       </c>
@@ -5451,7 +5450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>21332</v>
       </c>
@@ -5459,7 +5458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>39</v>
       </c>
@@ -5467,7 +5466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>21337</v>
       </c>
@@ -5475,7 +5474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>33</v>
       </c>
@@ -5483,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>21325</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>37</v>
       </c>
@@ -5499,7 +5498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>21330</v>
       </c>
@@ -5507,7 +5506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>41</v>
       </c>
@@ -5515,7 +5514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>21352</v>
       </c>
@@ -5523,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>35</v>
       </c>
@@ -5531,7 +5530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>21326</v>
       </c>
@@ -5539,7 +5538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>38</v>
       </c>
@@ -5547,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>21329</v>
       </c>
@@ -5555,7 +5554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>46</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>21361</v>
       </c>
@@ -5571,7 +5570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>13</v>
       </c>
@@ -5579,7 +5578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>43</v>
       </c>
@@ -5587,7 +5586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>21357</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>44</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>21358</v>
       </c>
@@ -5611,7 +5610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>14</v>
       </c>
@@ -5619,7 +5618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>47</v>
       </c>
@@ -5627,7 +5626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>21362</v>
       </c>
@@ -5635,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>48</v>
       </c>
@@ -5643,7 +5642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>21364</v>
       </c>
@@ -5651,7 +5650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>51</v>
       </c>
@@ -5659,7 +5658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>21367</v>
       </c>
@@ -5667,7 +5666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>60</v>
       </c>
@@ -5675,7 +5674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="8">
         <v>21368</v>
       </c>
@@ -5683,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>17</v>
       </c>
@@ -5691,7 +5690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>54</v>
       </c>
@@ -5699,7 +5698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>21371</v>
       </c>
@@ -5707,7 +5706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>53</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="8">
         <v>21369</v>
       </c>
@@ -5723,7 +5722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>52</v>
       </c>
@@ -5731,7 +5730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="8">
         <v>21370</v>
       </c>
@@ -5739,7 +5738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>58</v>
       </c>

</xml_diff>